<commit_message>
Big overhaul, new notebook copy, head 30 output
</commit_message>
<xml_diff>
--- a/data/EXECoutput.xlsx
+++ b/data/EXECoutput.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A80"/>
+  <dimension ref="A1:B78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,20 +436,22 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Point</t>
+          <t>Number</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Text</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Executive Summary
-INTRODUCTION</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>Health “is a state of complete physical, 
 mental and social well-being and 
@@ -461,8 +463,13 @@
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>Biological diversity  (biodiversity) is “the 
 variability among living organisms from 
@@ -476,8 +483,13 @@
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>Biodiversity underpins ecosystem 
 functioning and the provision of goods and services that are essential to human health and well-being. Ecosystems, 
@@ -487,8 +499,13 @@
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>The links between biodiversity and 
 health are manifested at various spatial and temporal scales. At a planetary scale, 
@@ -502,8 +519,13 @@
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>Biodiversity and human health, and 
 the respective policies and activities, 
@@ -523,8 +545,13 @@
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>Direct drivers of biodiversity loss include 
 land-use change, habitat loss, over-exploitation, pollution, invasive species and climate change. Many of these drivers aﬀect human health directly and through their impacts on biodiversity. The 
@@ -539,8 +566,13 @@
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>Human population health is determined, 
 to a large extent, by social, economic and 
@@ -553,8 +585,13 @@
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>Women and men have diﬀerent roles in the 
 conservation and use of biodiversity and varying health impacts. Access to, use, and 
@@ -562,8 +599,13 @@
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>The social and natural sciences are 
 important contributors to biodiversity 
@@ -588,8 +630,13 @@
         </is>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>Ecosystems provide clean water that 
 underpin many aspects of human health. 
@@ -599,8 +646,13 @@
         </is>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>Freshwater ecosystems, such as rivers, lakes 
 and wetlands, face disproportionately high 
@@ -615,8 +667,13 @@
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>Impaired water quality results in 
 significant social and economic costs.  
@@ -632,8 +689,13 @@
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>Water-related infrastructure has positive 
 and negative impacts on biodiversity, 
@@ -645,22 +707,20 @@
 illnesses such as schistosomiasis. Approaches integrating beneﬁts of both physical/built and natural infrastructure can provide more sustainable and cost-eﬀective solutions.
 Air pollution is one of the most significant 
 environmental health risks worldwide, responsible for 
-seven million deaths in 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Bronchial asthma and 
+seven million deaths in 2012. Bronchial asthma and 
 chronic obstructive pulmonary disease are on the rise. 
 Cardiovascular disease, immune disorders, various cancers, and disorders of the eye, ear, nose and throat 
 are also aﬀected by air pollution. Air pollution also aﬀects biodiversity; it can reduce plant biodiversity and aﬀect other ecosystem services, such as clean water and carbon storage.</t>
         </is>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>Ecosystems may aﬀect air quality and have 
 primarily beneﬁcial outcomes for human 
@@ -674,8 +734,13 @@
         </is>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
         <is>
           <t>Components of biodiversity can be used 
 as bioindicators of known human health 
@@ -695,8 +760,13 @@
         </is>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>Biodiversity in and around agricultural 
 production systems makes essential 
@@ -709,8 +779,13 @@
         </is>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
         <is>
           <t>The loss of diversity from agro-ecosystems 
 is increasing the vulnerability and reducing 
@@ -723,8 +798,13 @@
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
         <is>
           <t>The use of chemical inputs, particularly 
 pesticides, has had severe negative consequences for wildlife, human health and for agricultural biodiversity. While 
@@ -735,8 +815,13 @@
         </is>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
         <is>
           <t>Po llination is essential to food security 
 generally and to the production of many 
@@ -747,8 +832,13 @@
         </is>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
         <is>
           <t>Increas ing sustainable production and 
 meeting the challenges associated with climate change will require the increased use of agricultural biodiversity. Climate change is already having an impact the nutritional quality and safety of food and increasing the vulnerability of food insecure individuals and households. The increased use of agricultural biodiversity will play an 
@@ -758,8 +848,13 @@
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
         <is>
           <t>Agricultural practices, which make 
 improved use of agricultural biodiversity, have been identiﬁed and are being used 
@@ -785,8 +880,13 @@
         </is>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
         <is>
           <t>Access to wildlife in terrestrial, marine, 
 and freshwater systems is critical to 
@@ -797,8 +897,13 @@
         </is>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
         <is>
           <t>The harvest ing and trade of wild edible 
 plants and animals provides additional beneﬁts but also risks.  The collection and 
@@ -813,8 +918,13 @@
         </is>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
         <is>
           <t>Food based approaches are needed to 
 help combat malnutrition and promote health. A healthy, balanced diet requires a variety of foods to supply the full range of nutrients needed (vitamins, minerals, individual amino acids and fatty acids, and other beneﬁcial bioactive food components)  While fortiﬁcation and bio-fortiﬁcation may be cost-eﬀective solutions to address speciﬁc nutrient deficiencies (e.g. vitamin A and iron), they cannot provide the full range of nutrients needed. Food based approaches can be supported by a greater focus on nutrition and biological diversity in agricultural, food system and value chain programs and policies 
@@ -823,8 +933,13 @@
         </is>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
         <is>
           <t>Some dietary patterns that oﬀer substantial 
 health beneﬁts could also reduce climate change and pressures on biodiversity. The 
@@ -844,8 +959,13 @@
         </is>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
         <is>
           <t>Humans, like all complex plants and animals 
 have microbiota without which they could 
@@ -857,8 +977,13 @@
         </is>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
         <is>
           <t>Environmental  microbial ecosystems are 
 in constant dialogue and interchange with the human symbiotic ecosystems.   
@@ -874,8 +999,13 @@
         </is>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
         <is>
           <t>Several categories of org anism with 
 which we co-evolved play a role in setting up the mechanisms that “police” and regulate the immune system . In addition 
@@ -893,8 +1023,13 @@
         </is>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
         <is>
           <t>Reduced contact of people with the 
 natural environment and biodiversity and 
@@ -910,8 +1045,13 @@
         </is>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
         <is>
           <t>Failing immunoregulatory mechanisms 
 partly attributable to reduced contact with the natural environment and biodiversity lead to poor control of background inﬂammation . In high-income 
@@ -919,8 +1059,13 @@
         </is>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
         <is>
           <t>Understanding the factors that inﬂuence 
 functional and compositional changes in the human microbiome can contribute to 
@@ -935,8 +1080,13 @@
         </is>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
         <is>
           <t>Innovative design of cities and dwellings 
 m i g h t  b e  a b l e  t o  i n c r e a s e  e x p o s u r e  t o  the microbial biodiversity that our physiological systems have evolved to expect . In high-income settings several very 
@@ -944,8 +1094,13 @@
         </is>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
         <is>
           <t>Consider ing “microbial diversity” as 
 an ecosystem service provider may contribute to bridging the chasm between ecology and medicine/immunology, by considering microbial diversity in public health and conservation strategies aimed at maximizing services obtained from ecosystems.  The relationships our individual 
@@ -963,8 +1118,13 @@
         </is>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
         <is>
           <t>Pathog ens play a complex role in 
 biodiversity and health, with beneﬁts in 
@@ -975,8 +1135,13 @@
         </is>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
         <is>
           <t>Human-caused c hanges in ecosystems, 
 such as modified landscapes, intensive agriculture, and antimicrobial use, are 
@@ -991,8 +1156,13 @@
         </is>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
         <is>
           <t>Areas of high biodiversity may have high 
 numbers of pathogens, yet biodiversity may serve as a protective factor for 
@@ -1007,8 +1177,13 @@
         </is>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
         <is>
           <t>Infectious diseases threaten wild species 
 as well as the people that depend on them. 
@@ -1024,8 +1199,13 @@
         </is>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
         <is>
           <t>The rapidly grow ing number of invasive 
 species cause signiﬁcant impacts on human 
@@ -1047,8 +1227,13 @@
         </is>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
         <is>
           <t>Biodiversity has been an irreplaceable 
 resource for the discovery of medicines 
@@ -1058,8 +1243,13 @@
         </is>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
         <is>
           <t>For many of the most challenging health 
 problems facing humanity today, we look to 
@@ -1075,8 +1265,13 @@
         </is>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
         <is>
           <t>Greater even than what individual species 
 offer to medicine through molecules 
@@ -1092,8 +1287,13 @@
         </is>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
         <is>
           <t>Traditional medical knowledge spans 
 various dimensions relating to medicines, 
@@ -1106,8 +1306,13 @@
         </is>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
         <is>
           <t>Medicinal and aromatic plants, the great 
 majority of which are sourced from the wild, are used in traditional medicine and also in the pharmaceutical, cosmetic and food industries.  The global use and trade 
@@ -1121,8 +1326,13 @@
         </is>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
         <is>
           <t>Threats to medicinal plants, animals and 
 other medicinal resources are increasing. Wild plant populations are declining-  one in 
@@ -1137,8 +1347,13 @@
         </is>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
         <is>
           <t>Sustainable use of medicinal resources can 
 provide multiple beneﬁts to biodiversity, 
@@ -1157,8 +1372,13 @@
         </is>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
         <is>
           <t>Sui generis mod els may need to be 
 developed and applied to secure rights of 
@@ -1168,8 +1388,13 @@
         </is>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
         <is>
           <t>Improv ing public health outcomes and 
 achieving objectives of ‘Health for All’ and ‘Good Health at Low Cost’ should include traditional medical care and the development of appropriate integrative methodologies and safety standards within and across medical systems. More than one-third of the population in many developing countries do not have access to modern healthcare, and are dependent on traditional medical systems. There is a high patronage of and dependence on traditional health practitioners to provide care to people with inadequate access to modern health infrastructure or with a preference for traditional systems. Pluralistic approaches that integrate natural resources and medical knowledge and are sensitive to local priorities and contexts can enable better health outcomes. This implies the need to develop cross-sectoral, cost-effective measures to test safety, eﬃcacy and quality of traditional medicines, the integration of traditional healers in the healthcare system through appropriate accreditation practices and processes, cross-learning between diﬀerent knowledge systems and disciplines through participatory, formal and informal learning processes to supplement current practices in a culturally sensitive way.
@@ -1183,8 +1408,13 @@
         </is>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
         <is>
           <t>The interaction with nature – inclu ding 
 domestic animals, and wild animals in wild 
@@ -1198,8 +1428,13 @@
         </is>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
         <is>
           <t>Exposure to green space may have positive 
 impacts on mental health.  Depression 
@@ -1214,8 +1449,13 @@
         </is>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
         <is>
           <t>Access to natural green space can increase 
 levels of physical activity with beneﬁts for health. The beneﬁts of physical activity may include reduced risk of several non-communicable diseases, as well as improved immune function. It may also provide mental 
@@ -1231,8 +1471,13 @@
         </is>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
         <is>
           <t>Biodiversity is often central to cultures, 
 cultural traditions and cultural well-being. Species, habitats, ecosystems, and 
@@ -1245,8 +1490,13 @@
         </is>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
         <is>
           <t>Signiﬁcant changes to local biodiversity or 
 ecosystem sustainability can have speciﬁc and unique impacts on local community health where the physical health of a community is directly inﬂuenced by or dependent upon ecosystem services, particularly regarding access to diverse 
@@ -1257,8 +1507,13 @@
         </is>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
         <is>
           <t>While many community-specific links 
 between health, culture and biodiversity have been documented and measured, much of the evidence for a more universal relationship is relatively sparse beyond anecdotal accounts. However, there is 
@@ -1271,8 +1526,13 @@
         </is>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
         <is>
           <t>The release of pharmaceuticals and 
 Active Pharmaceutical Ingredients 
@@ -1284,8 +1544,13 @@
         </is>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
         <is>
           <t>Antibiotic and antimicrobial use can 
 alter the composition and function of the 
@@ -1302,8 +1567,13 @@
         </is>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
         <is>
           <t>The inappropriate use of antibiotics in 
 plants, animals, and humans has cultivated 
@@ -1327,8 +1597,13 @@
         </is>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
         <is>
           <t>Endocrine disrupting chemicals found in 
 pharmaceuticals products and also in many 
@@ -1344,8 +1619,13 @@
         </is>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
         <is>
           <t>The inappropriate use of some non-
 steroidal anti-inflammatory drugs and other veterinary drugs  threatens wildlife 
@@ -1365,8 +1645,13 @@
         </is>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>59</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
         <is>
           <t>Climate c hange is already negatively 
 impacting on human health and these 
@@ -1379,8 +1664,13 @@
         </is>
       </c>
     </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
         <is>
           <t>Climate c hange will not only affect 
 agricultural production systems but also the nutritional content of foods and the distribution and availability of ﬁsheries. Changes in temperature and precipitation patterns will have complex eﬀects, but the 
@@ -1391,8 +1681,13 @@
         </is>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
         <is>
           <t>Disasters may be precipitated by impacts 
 on critical ecosystems or the collapse of essential ecosystem services. Disasters 
@@ -1402,8 +1697,13 @@
         </is>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
         <is>
           <t>Competition over access to ecosystem 
 goods and services can contribute to, and become a cause of, conflict, with consequences that can negatively impact ecosystem goods and services in both the short- and long-term. Greater recognition 
@@ -1413,8 +1713,13 @@
         </is>
       </c>
     </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
         <is>
           <t>The creation of disaster-resilient societies 
 is increasingly tied to and dependent upon 
@@ -1430,8 +1735,13 @@
         </is>
       </c>
     </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
         <is>
           <t>Biodiversity helps to improve resilience of 
 ecosystems, contributing to adaptation to 
@@ -1446,8 +1756,13 @@
         </is>
       </c>
     </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
         <is>
           <t>Increased pressure on the biosphere, driven 
 by increasing human populations and per 
@@ -1462,8 +1777,13 @@
         </is>
       </c>
     </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
         <is>
           <t>Alternative scenario s to 2050, as well as 
 practical experience, demonstrate that it is 
@@ -1479,8 +1799,13 @@
         </is>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>67</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
         <is>
           <t>Behavioural change is needed to improve 
 human health and protect biodiversity. Human behaviour, which is informed by 
@@ -1495,8 +1820,13 @@
         </is>
       </c>
     </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
         <is>
           <t>Health and biodiversity strategies could be 
 developed with the aim of ensuring that 
@@ -1542,8 +1872,13 @@
         </is>
       </c>
     </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
         <is>
           <t>Integration of biodiversity and human 
 health concerns will require the use 
@@ -1556,8 +1891,13 @@
         </is>
       </c>
     </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
         <is>
           <t>The development of comparable tools–and 
 maximizing the use of existing tools–to promote a common evidence base across sectors is needed.  Tools ranging 
@@ -1567,8 +1907,13 @@
         </is>
       </c>
     </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
         <is>
           <t>The development of precautionary policies 
 that place a value on ecosystem services to 
@@ -1578,8 +1923,13 @@
         </is>
       </c>
     </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
         <is>
           <t>Measuring health effects of ecosystem 
 change considering established “exposure” 
@@ -1592,8 +1942,13 @@
         </is>
       </c>
     </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
         <is>
           <t>Economic valuation approaches linking 
 ecosystem functioning and health that 
@@ -1607,8 +1962,13 @@
         </is>
       </c>
     </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
         <is>
           <t>Further research is needed to elucidate 
 some of the potential knowledge gaps on linkages between biodiversity and human health. Examples of key questions include:a. What are the relationships between 
@@ -1622,8 +1982,13 @@
         </is>
       </c>
     </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
         <is>
           <t>Health and biodiversity, and the linkages 
 among them and with other elements 
@@ -1637,8 +2002,13 @@
         </is>
       </c>
     </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
         <is>
           <t>Ongo ing evaluation of synergistic and 
 antagonistic effects of complementary sustainable development goals and targets is needed.  This includes sustainable 
@@ -1650,8 +2020,13 @@
         </is>
       </c>
     </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
         <is>
           <t>Health is our most basic human right 
 and therefore one of the most important indicators of sustainable development. At the same time, the conservation and sustainable use of biodiversity is imperative for the continued functioning of ecosystems at all scales, and for the delivery of ecosystem services that are essential for human health . There are many 

</xml_diff>